<commit_message>
Template: Make template more generic
</commit_message>
<xml_diff>
--- a/luke_wip/Template.xlsx
+++ b/luke_wip/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\luke\SwimifyHandler\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\luke\SwimifyHandler\luke_wip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DC08F-2207-4259-9402-5EC1DDE60E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FD3D75-E5C6-40C3-BF6B-DA1F2094B563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32460" yWindow="2280" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty" sheetId="4" r:id="rId1"/>
@@ -184,13 +184,13 @@
     <t>30. 50m</t>
   </si>
   <si>
-    <t>HS</t>
-  </si>
-  <si>
-    <t>Swedish Swim Games 2024 - GP</t>
-  </si>
-  <si>
-    <t>20 September - 22 September (2024)</t>
+    <t>CLUB</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Rename sheet and remove artifacts from template after export
</commit_message>
<xml_diff>
--- a/luke_wip/Template.xlsx
+++ b/luke_wip/Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\luke\SwimifyHandler\luke_wip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FD3D75-E5C6-40C3-BF6B-DA1F2094B563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FCC56-1E44-4FEE-82C5-6EA187123BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32460" yWindow="2280" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31080" yWindow="3660" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Empty" sheetId="4" r:id="rId1"/>
+    <sheet name="Template" sheetId="4" r:id="rId1"/>
     <sheet name="25m" sheetId="11" r:id="rId2"/>
     <sheet name="50m" sheetId="5" r:id="rId3"/>
     <sheet name="100m" sheetId="6" r:id="rId4"/>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>